<commit_message>
old code only for ref
</commit_message>
<xml_diff>
--- a/jobs/queries.xlsx
+++ b/jobs/queries.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dc/db_load_test/jobs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dc/snow_test_suite/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DA7E82-1C5D-3F4D-B828-CDDCC26415EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC5FFC6E-75A9-AE49-B649-02BEAE6AC1F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{F1E7B76B-B87E-FE45-966D-41D60C1495F7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{F1E7B76B-B87E-FE45-966D-41D60C1495F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>qid</t>
   </si>
@@ -49,79 +48,34 @@
     <t>report_name</t>
   </si>
   <si>
+    <t>r_comparison_caterpillar</t>
+  </si>
+  <si>
+    <t>r_sub_details_accepted_cases</t>
+  </si>
+  <si>
+    <t>r_submission_details_first_quadrant</t>
+  </si>
+  <si>
+    <t>select * from a where id = $PARAM1</t>
+  </si>
+  <si>
+    <t>select * from a where id = $PARAM1 and name = $PARAM2</t>
+  </si>
+  <si>
+    <t>select * from c where id = $PARAM1 and name = $PARAM2 and age = $PARAM3</t>
+  </si>
+  <si>
+    <t>17184,15660,16063,15705,16096,15656,15770,15539,15613,15738</t>
+  </si>
+  <si>
+    <t>3,4,5,6,7,8,9,10</t>
+  </si>
+  <si>
     <t>param3</t>
   </si>
   <si>
-    <t>3,4</t>
-  </si>
-  <si>
-    <t>database</t>
-  </si>
-  <si>
-    <t>host</t>
-  </si>
-  <si>
-    <t>port</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>pwd</t>
-  </si>
-  <si>
-    <t>ROLE</t>
-  </si>
-  <si>
-    <t>WH</t>
-  </si>
-  <si>
-    <t>SCHEMA</t>
-  </si>
-  <si>
-    <t>DATABASE</t>
-  </si>
-  <si>
-    <t>table_name</t>
-  </si>
-  <si>
-    <t>Filename</t>
-  </si>
-  <si>
-    <t>Run_name</t>
-  </si>
-  <si>
-    <t>Number_of_runs</t>
-  </si>
-  <si>
-    <t>qids</t>
-  </si>
-  <si>
-    <t>total runs</t>
-  </si>
-  <si>
-    <t>Total time</t>
-  </si>
-  <si>
-    <t>1,2,3,4</t>
-  </si>
-  <si>
-    <t>1002, 1143, 1102</t>
-  </si>
-  <si>
-    <t>r_customer</t>
-  </si>
-  <si>
-    <t>r_employee</t>
-  </si>
-  <si>
-    <t>select * from customers where customer_id = $PARAM1</t>
-  </si>
-  <si>
-    <t>23,27,73</t>
-  </si>
-  <si>
-    <t>select * from employees where manager_id = $PARAM1 and job_title in ($PARAM2:3#)</t>
+    <t>99,77,88,99</t>
   </si>
 </sst>
 </file>
@@ -157,16 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +434,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,7 +442,7 @@
     <col min="2" max="2" width="38.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="89.83203125" customWidth="1"/>
     <col min="4" max="4" width="57" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -512,7 +462,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -520,16 +470,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -537,106 +487,36 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1794890-5236-BB4D-8DD1-1A17EC5AF73A}">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="F4" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>